<commit_message>
updated excel & deleted in from notepad
</commit_message>
<xml_diff>
--- a/departments_2023-10-19_04_26_14.xlsx
+++ b/departments_2023-10-19_04_26_14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Payel\Ralvie234\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0E3C2A-23D2-4A20-880E-81A8E1DE4D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7486C1A-8E5B-4434-922E-9BE835243442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="1371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="1370">
   <si>
     <t>Department Name*(mandatory)</t>
   </si>
@@ -4130,9 +4130,6 @@
   </si>
   <si>
     <t>DEPT2019</t>
-  </si>
-  <si>
-    <t>DEPT2019246</t>
   </si>
 </sst>
 </file>
@@ -4505,8 +4502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1350" workbookViewId="0">
-      <selection activeCell="C1366" sqref="C1366"/>
+    <sheetView tabSelected="1" topLeftCell="A1353" workbookViewId="0">
+      <selection activeCell="A1367" sqref="A1367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15450,7 +15447,7 @@
     </row>
     <row r="1367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1367" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B1367" t="s">
         <v>1369</v>

</xml_diff>